<commit_message>
Fazendo o front com template engine em GO
</commit_message>
<xml_diff>
--- a/Books.xlsx
+++ b/Books.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="211">
   <si>
     <t>Storytelling com dados: um guia sobre visualização de dados para profissionais de negócios</t>
   </si>
@@ -26,7 +26,7 @@
     <t>R$ 79,63</t>
   </si>
   <si>
-    <t>amazon.com.br/Storytelling-com-Dados-Visualiza%C3%A7%C3%A3o-Profissionais/dp/8550804681/ref=zg_mw_g_7842670011_sccl_1/145-7952979-0205767?psc=1</t>
+    <t>amazon.com.br/Storytelling-com-Dados-Visualiza%C3%A7%C3%A3o-Profissionais/dp/8550804681/ref=zg_mw_g_7842670011_sccl_1/136-2212818-9687203?psc=1</t>
   </si>
   <si>
     <t>Código limpo: habilidades práticas do Agile software</t>
@@ -35,10 +35,10 @@
     <t>Robert C. Martin</t>
   </si>
   <si>
-    <t>R$ 100,26</t>
-  </si>
-  <si>
-    <t>amazon.com.br/C%C3%B3digo-limpo-Robert-C-Martin/dp/8576082675/ref=zg_mw_g_7842670011_sccl_2/145-7952979-0205767?psc=1</t>
+    <t>R$ 101,69</t>
+  </si>
+  <si>
+    <t>amazon.com.br/C%C3%B3digo-limpo-Robert-C-Martin/dp/8576082675/ref=zg_mw_g_7842670011_sccl_2/136-2212818-9687203?psc=1</t>
   </si>
   <si>
     <t>Data science do zero: primeiras regras com o Python</t>
@@ -50,7 +50,7 @@
     <t>R$ 61,52</t>
   </si>
   <si>
-    <t>amazon.com.br/Data-Science-zero-Joel-Grus/dp/857608998X/ref=zg_mw_g_7842670011_sccl_3/145-7952979-0205767?psc=1</t>
+    <t>amazon.com.br/Data-Science-zero-Joel-Grus/dp/857608998X/ref=zg_mw_g_7842670011_sccl_3/136-2212818-9687203?psc=1</t>
   </si>
   <si>
     <t>Estatística prática para cientistas de dados: 50 conceitos essenciaisAndrew Bruce</t>
@@ -62,7 +62,7 @@
     <t>R$ 87,89</t>
   </si>
   <si>
-    <t>amazon.com.br/Estat%C3%ADstica-Pr%C3%A1tica-Para-Cientistas-Dados/dp/855080603X/ref=zg_mw_g_7842670011_sccl_4/145-7952979-0205767?psc=1</t>
+    <t>amazon.com.br/Estat%C3%ADstica-Pr%C3%A1tica-Para-Cientistas-Dados/dp/855080603X/ref=zg_mw_g_7842670011_sccl_4/136-2212818-9687203?psc=1</t>
   </si>
   <si>
     <t>Python Fluente: Programação Clara, Concisa e Eficaz</t>
@@ -74,7 +74,7 @@
     <t>R$ 159,00</t>
   </si>
   <si>
-    <t>amazon.com.br/Python-Fluente-Programa%C3%A7%C3%A3o-Concisa-Eficaz/dp/857522462X/ref=zg_mw_g_7842670011_sccl_5/145-7952979-0205767?psc=1</t>
+    <t>amazon.com.br/Python-Fluente-Programa%C3%A7%C3%A3o-Concisa-Eficaz/dp/857522462X/ref=zg_mw_g_7842670011_sccl_5/136-2212818-9687203?psc=1</t>
   </si>
   <si>
     <t>Scrum e Métodos Ágeis: Um Guia Prático</t>
@@ -86,7 +86,7 @@
     <t>R$ 12,99</t>
   </si>
   <si>
-    <t>amazon.com.br/Scrum-M%C3%A9todos-%C3%81geis-Guia-Pr%C3%A1tico-ebook/dp/B01LBSPIAG/ref=zg_mw_g_7842670011_sccl_6/145-7952979-0205767?psc=1</t>
+    <t>amazon.com.br/Scrum-M%C3%A9todos-%C3%81geis-Guia-Pr%C3%A1tico-ebook/dp/B01LBSPIAG/ref=zg_mw_g_7842670011_sccl_6/136-2212818-9687203?psc=1</t>
   </si>
   <si>
     <t>Domain-driven design: atacando as complexidades no coração do software</t>
@@ -98,7 +98,7 @@
     <t>R$ 100,75</t>
   </si>
   <si>
-    <t>amazon.com.br/Domain-driven-design-atacando-complexidades-software/dp/8550800651/ref=zg_mw_g_7842670011_sccl_7/145-7952979-0205767?psc=1</t>
+    <t>amazon.com.br/Domain-driven-design-atacando-complexidades-software/dp/8550800651/ref=zg_mw_g_7842670011_sccl_7/136-2212818-9687203?psc=1</t>
   </si>
   <si>
     <t>Algoritmos para viver - A ciência exata das decisões humanasBrian Christian &amp; Tom Griffiths</t>
@@ -110,7 +110,7 @@
     <t>R$ 56,98</t>
   </si>
   <si>
-    <t>amazon.com.br/Algoritmos-para-viver-ci%C3%AAncia-decis%C3%B5es/dp/8535929304/ref=zg_mw_g_7842670011_sccl_8/145-7952979-0205767?psc=1</t>
+    <t>amazon.com.br/Algoritmos-para-viver-ci%C3%AAncia-decis%C3%B5es/dp/8535929304/ref=zg_mw_g_7842670011_sccl_8/136-2212818-9687203?psc=1</t>
   </si>
   <si>
     <t>Python: Guia prático do básico ao avançado (Cientista de dados Livro 2)</t>
@@ -122,7 +122,7 @@
     <t>R$ 5,99</t>
   </si>
   <si>
-    <t>amazon.com.br/Python-pr%C3%A1tico-b%C3%A1sico-avan%C3%A7ado-Cientista-ebook/dp/B07KML8M9L/ref=zg_mw_g_7842670011_sccl_9/145-7952979-0205767?psc=1</t>
+    <t>amazon.com.br/Python-pr%C3%A1tico-b%C3%A1sico-avan%C3%A7ado-Cientista-ebook/dp/B07KML8M9L/ref=zg_mw_g_7842670011_sccl_9/136-2212818-9687203?psc=1</t>
   </si>
   <si>
     <t>Entendendo Algoritmos: Um Guia Ilustrado Para Programadores e Outros CuriososAditya Y. Bhargava</t>
@@ -134,7 +134,7 @@
     <t>R$ 65,54</t>
   </si>
   <si>
-    <t>amazon.com.br/Entendendo-Algoritmos-Ilustrado-Programadores-Curiosos/dp/8575225634/ref=zg_mw_g_7842670011_sccl_10/145-7952979-0205767?psc=1</t>
+    <t>amazon.com.br/Entendendo-Algoritmos-Ilustrado-Programadores-Curiosos/dp/8575225634/ref=zg_mw_g_7842670011_sccl_10/136-2212818-9687203?psc=1</t>
   </si>
   <si>
     <t>Introdução à Programação com Python: Algoritmos e Lógica de Programação Para Iniciantes</t>
@@ -143,10 +143,10 @@
     <t>Nilo Ney Coutinho Menezes</t>
   </si>
   <si>
-    <t>R$ 79,74</t>
-  </si>
-  <si>
-    <t>amazon.com.br/Introdu%C3%A7%C3%A3o-Programa%C3%A7%C3%A3o-com-Python-Algoritmos/dp/8575227181/ref=zg_mw_g_7842670011_sccl_11/145-7952979-0205767?psc=1</t>
+    <t>R$ 79,89</t>
+  </si>
+  <si>
+    <t>amazon.com.br/Introdu%C3%A7%C3%A3o-Programa%C3%A7%C3%A3o-com-Python-Algoritmos/dp/8575227181/ref=zg_mw_g_7842670011_sccl_11/136-2212818-9687203?psc=1</t>
   </si>
   <si>
     <t>O codificador limpo: um código de conduta para programadores profissionaisBob Martin</t>
@@ -158,7 +158,7 @@
     <t>R$ 56,99</t>
   </si>
   <si>
-    <t>amazon.com.br/codificador-limpo-conduta-programadores-profissionais/dp/8576086476/ref=zg_mw_g_7842670011_sccl_12/145-7952979-0205767?psc=1</t>
+    <t>amazon.com.br/codificador-limpo-conduta-programadores-profissionais/dp/8576086476/ref=zg_mw_g_7842670011_sccl_12/136-2212818-9687203?psc=1</t>
   </si>
   <si>
     <t>Mãos à obra: aprendizado de máquina com scikit-learn &amp; tensorflow</t>
@@ -170,7 +170,7 @@
     <t>R$ 90,09</t>
   </si>
   <si>
-    <t>amazon.com.br/M%C3%A3os-obra-aprendizado-scikit-learn-tensorflow/dp/8550803812/ref=zg_mw_g_7842670011_sccl_13/145-7952979-0205767?psc=1</t>
+    <t>amazon.com.br/M%C3%A3os-obra-aprendizado-scikit-learn-tensorflow/dp/8550803812/ref=zg_mw_g_7842670011_sccl_13/136-2212818-9687203?psc=1</t>
   </si>
   <si>
     <t>O mítico homem-mês: ensaios sobre engenharia de softwareFrederick P. Brooks Jr.</t>
@@ -179,10 +179,10 @@
     <t>Frederick P. Brooks Jr.</t>
   </si>
   <si>
-    <t>R$ 84,98</t>
-  </si>
-  <si>
-    <t>amazon.com.br/m%C3%ADtico-homem-m%C3%AAs-ensaios-engenharia-software/dp/8550802530/ref=zg_mw_g_7842670011_sccl_14/145-7952979-0205767?psc=1</t>
+    <t>R$ 84,26</t>
+  </si>
+  <si>
+    <t>amazon.com.br/m%C3%ADtico-homem-m%C3%AAs-ensaios-engenharia-software/dp/8550802530/ref=zg_mw_g_7842670011_sccl_14/136-2212818-9687203?psc=1</t>
   </si>
   <si>
     <t>Padrões de Projetos: Soluções Reutilizáveis de Software Orientados a Objetos</t>
@@ -194,7 +194,7 @@
     <t>R$ 162,46</t>
   </si>
   <si>
-    <t>amazon.com.br/Padr%C3%B5es-Projetos-Solu%C3%A7%C3%B5es-Reutiliz%C3%A1veis-Orientados/dp/8573076100/ref=zg_mw_g_7842670011_sccl_15/145-7952979-0205767?psc=1</t>
+    <t>amazon.com.br/Padr%C3%B5es-Projetos-Solu%C3%A7%C3%B5es-Reutiliz%C3%A1veis-Orientados/dp/8573076100/ref=zg_mw_g_7842670011_sccl_15/136-2212818-9687203?psc=1</t>
   </si>
   <si>
     <t>Curso Intensivo de Python: Uma Introdução Prática e Baseada em Projetos à Programação</t>
@@ -206,7 +206,7 @@
     <t>R$ 380,00</t>
   </si>
   <si>
-    <t>amazon.com.br/Curso-Intensivo-Python-Introdu%C3%A7%C3%A3o-Programa%C3%A7%C3%A3o/dp/8575225030/ref=zg_mw_g_7842670011_sccl_16/145-7952979-0205767?psc=1</t>
+    <t>amazon.com.br/Curso-Intensivo-Python-Introdu%C3%A7%C3%A3o-Programa%C3%A7%C3%A3o/dp/8575225030/ref=zg_mw_g_7842670011_sccl_16/136-2212818-9687203?psc=1</t>
   </si>
   <si>
     <t>Sprint a Sprint: Erros e acertos na transformação cultural de um time ágil</t>
@@ -218,7 +218,7 @@
     <t>R$ 18,37</t>
   </si>
   <si>
-    <t>amazon.com.br/Sprint-Erros-acertos-transforma%C3%A7%C3%A3o-cultural-ebook/dp/B087N2LKXB/ref=zg_mw_g_7842670011_sccl_17/145-7952979-0205767?psc=1</t>
+    <t>amazon.com.br/Sprint-Erros-acertos-transforma%C3%A7%C3%A3o-cultural-ebook/dp/B087N2LKXB/ref=zg_mw_g_7842670011_sccl_17/136-2212818-9687203?psc=1</t>
   </si>
   <si>
     <t>Sangue, suor e pixels: Os dramas, as vitórias e as curiosas histórias por trás dos videogames</t>
@@ -230,7 +230,7 @@
     <t>R$ 49,90</t>
   </si>
   <si>
-    <t>amazon.com.br/Sangue-Suor-Pixels-Jason-Schreier/dp/8595082596/ref=zg_mw_g_7842670011_sccl_18/145-7952979-0205767?psc=1</t>
+    <t>amazon.com.br/Sangue-Suor-Pixels-Jason-Schreier/dp/8595082596/ref=zg_mw_g_7842670011_sccl_18/136-2212818-9687203?psc=1</t>
   </si>
   <si>
     <t>Pense em Python: Pense Como um Cientista da ComputaçãoAllen B. Downey</t>
@@ -242,7 +242,7 @@
     <t>R$ 81,64</t>
   </si>
   <si>
-    <t>amazon.com.br/Pense-Python-Como-Cientista-Computa%C3%A7%C3%A3o/dp/8575225081/ref=zg_mw_g_7842670011_sccl_20/145-7952979-0205767?psc=1</t>
+    <t>amazon.com.br/Pense-Python-Como-Cientista-Computa%C3%A7%C3%A3o/dp/8575225081/ref=zg_mw_g_7842670011_sccl_20/136-2212818-9687203?psc=1</t>
   </si>
   <si>
     <t>Programação Web com Node.js: Completo, do Front-end ao Back-end</t>
@@ -251,7 +251,7 @@
     <t>R$ 14,99</t>
   </si>
   <si>
-    <t>amazon.com.br/Programa%C3%A7%C3%A3o-Web-com-Node-js-Front-end-ebook/dp/B074RCRKSL/ref=zg_mw_g_7842670011_sccl_21/145-7952979-0205767?psc=1</t>
+    <t>amazon.com.br/Programa%C3%A7%C3%A3o-Web-com-Node-js-Front-end-ebook/dp/B074RCRKSL/ref=zg_mw_g_7842670011_sccl_21/136-2212818-9687203?psc=1</t>
   </si>
   <si>
     <t>Lean Inception: Como alinhar pessoas e construir o produto certo</t>
@@ -263,7 +263,7 @@
     <t>R$ 67,89</t>
   </si>
   <si>
-    <t>amazon.com.br/Lean-Inception-Alinhar-Pessoas-Construir/dp/8594377061/ref=zg_mw_g_7842670011_sccl_22/145-7952979-0205767?psc=1</t>
+    <t>amazon.com.br/Lean-Inception-Alinhar-Pessoas-Construir/dp/8594377061/ref=zg_mw_g_7842670011_sccl_22/136-2212818-9687203?psc=1</t>
   </si>
   <si>
     <t>Plataforma: a revolução da estratégiaGeoffrey G. Parker</t>
@@ -275,7 +275,7 @@
     <t>R$ 50,99</t>
   </si>
   <si>
-    <t>amazon.com.br/Plataforma-Revolu%C3%A7%C3%A3o-Estrat%C3%A9gia-Geoffrey-Parker/dp/8550806137/ref=zg_mw_g_7842670011_sccl_23/145-7952979-0205767?psc=1</t>
+    <t>amazon.com.br/Plataforma-Revolu%C3%A7%C3%A3o-Estrat%C3%A9gia-Geoffrey-Parker/dp/8550806137/ref=zg_mw_g_7842670011_sccl_23/136-2212818-9687203?psc=1</t>
   </si>
   <si>
     <t>O Algoritmo Mestre: Como a Busca Pelo Algoritmo de Machine Learning Definitivo Recriará Nosso Mundo</t>
@@ -284,10 +284,7 @@
     <t>Pedro Domingos</t>
   </si>
   <si>
-    <t>R$ 79,89</t>
-  </si>
-  <si>
-    <t>amazon.com.br/Algoritmo-Mestre-Learning-Definitivo-Recriar%C3%A1/dp/8575225383/ref=zg_mw_g_7842670011_sccl_24/145-7952979-0205767?psc=1</t>
+    <t>amazon.com.br/Algoritmo-Mestre-Learning-Definitivo-Recriar%C3%A1/dp/8575225383/ref=zg_mw_g_7842670011_sccl_24/136-2212818-9687203?psc=1</t>
   </si>
   <si>
     <t>Python Aplicado: Bolsa de Valores - Um guia para construção de análises e indicadores</t>
@@ -299,13 +296,13 @@
     <t>R$ 24,90</t>
   </si>
   <si>
-    <t>amazon.com.br/Python-Aplicado-constru%C3%A7%C3%A3o-an%C3%A1lises-indicadores-ebook/dp/B07QNDC8CL/ref=zg_mw_g_7842670011_sccl_25/145-7952979-0205767?psc=1</t>
+    <t>amazon.com.br/Python-Aplicado-constru%C3%A7%C3%A3o-an%C3%A1lises-indicadores-ebook/dp/B07QNDC8CL/ref=zg_mw_g_7842670011_sccl_25/136-2212818-9687203?psc=1</t>
   </si>
   <si>
     <t>R$ 24,87</t>
   </si>
   <si>
-    <t>amazon.com.br/Sangue-suor-pixels-hist%C3%B3rias-videogames-ebook/dp/B07BWM2LB9/ref=zg_mw_g_7842670011_sccl_27/145-7952979-0205767?psc=1</t>
+    <t>amazon.com.br/Sangue-suor-pixels-hist%C3%B3rias-videogames-ebook/dp/B07BWM2LB9/ref=zg_mw_g_7842670011_sccl_27/136-2212818-9687203?psc=1</t>
   </si>
   <si>
     <t>Métricas Ágeis: Obtenha melhores resultados em sua equipeRaphael Donaire Albino</t>
@@ -314,7 +311,7 @@
     <t>Raphael Donaire Albino</t>
   </si>
   <si>
-    <t>amazon.com.br/M%C3%A9tricas-%C3%81geis-Obtenha-melhores-resultados-ebook/dp/B072MHLBH1/ref=zg_mw_g_7842670011_sccl_29/145-7952979-0205767?psc=1</t>
+    <t>amazon.com.br/M%C3%A9tricas-%C3%81geis-Obtenha-melhores-resultados-ebook/dp/B072MHLBH1/ref=zg_mw_g_7842670011_sccl_29/136-2212818-9687203?psc=1</t>
   </si>
   <si>
     <t>Web Scraping com Python: Coletando Mais Dados da web Moderna</t>
@@ -326,7 +323,7 @@
     <t>R$ 82,89</t>
   </si>
   <si>
-    <t>amazon.com.br/Web-Scraping-Com-Python-Coletando/dp/8575227300/ref=zg_mw_g_7842670011_sccl_30/145-7952979-0205767?psc=1</t>
+    <t>amazon.com.br/Web-Scraping-Com-Python-Coletando/dp/8575227300/ref=zg_mw_g_7842670011_sccl_30/136-2212818-9687203?psc=1</t>
   </si>
   <si>
     <t>Automatize Tarefas Maçantes com Python: Programação Prática Para Verdadeiros Iniciantes</t>
@@ -350,7 +347,7 @@
     <t>R$ 109,74</t>
   </si>
   <si>
-    <t>amazon.com.br/Programa%C3%A7%C3%A3o-Baixo-N%C3%ADvel-Programas-Arquitetura/dp/8575226673/ref=zg_mw_g_7842670011_sccl_1/145-7952979-0205767?psc=1</t>
+    <t>amazon.com.br/Programa%C3%A7%C3%A3o-Baixo-N%C3%ADvel-Programas-Arquitetura/dp/8575226673/ref=zg_mw_g_7842670011_sccl_1/136-2212818-9687203?psc=1</t>
   </si>
   <si>
     <t>Introdução à Linguagem SQL: Abordagem Prática Para Iniciantes</t>
@@ -362,7 +359,7 @@
     <t>R$ 54,49</t>
   </si>
   <si>
-    <t>amazon.com.br/Introdu%C3%A7%C3%A3o-Linguagem-SQL-Abordagem-Iniciantes/dp/8575225014/ref=zg_mw_g_7842670011_sccl_2/145-7952979-0205767?psc=1</t>
+    <t>amazon.com.br/Introdu%C3%A7%C3%A3o-Linguagem-SQL-Abordagem-Iniciantes/dp/8575225014/ref=zg_mw_g_7842670011_sccl_2/136-2212818-9687203?psc=1</t>
   </si>
   <si>
     <t>Engenharia de Confiabilidade do Google: Como o Google Administra Seus Sistemas de Produção</t>
@@ -374,7 +371,7 @@
     <t>R$ 135,49</t>
   </si>
   <si>
-    <t>amazon.com.br/Engenharia-Confiabilidade-Google-Administra-Sistemas/dp/8575225170/ref=zg_mw_g_7842670011_sccl_3/145-7952979-0205767?psc=1</t>
+    <t>amazon.com.br/Engenharia-Confiabilidade-Google-Administra-Sistemas/dp/8575225170/ref=zg_mw_g_7842670011_sccl_3/136-2212818-9687203?psc=1</t>
   </si>
   <si>
     <t>JavaScript: O Guia Definitivo</t>
@@ -386,13 +383,13 @@
     <t>R$ 225,41</t>
   </si>
   <si>
-    <t>amazon.com.br/JavaScript-Guia-Definitivo-David-Flanagan/dp/856583719X/ref=zg_mw_g_7842670011_sccl_4/145-7952979-0205767?psc=1</t>
+    <t>amazon.com.br/JavaScript-Guia-Definitivo-David-Flanagan/dp/856583719X/ref=zg_mw_g_7842670011_sccl_4/136-2212818-9687203?psc=1</t>
   </si>
   <si>
     <t>R$ 187,20</t>
   </si>
   <si>
-    <t>amazon.com.br/JavaScript-Guia-Definitivo-David-Flanagan-ebook/dp/B016N7G8EK/ref=zg_mw_g_7842670011_sccl_5/145-7952979-0205767?psc=1</t>
+    <t>amazon.com.br/JavaScript-Guia-Definitivo-David-Flanagan-ebook/dp/B016N7G8EK/ref=zg_mw_g_7842670011_sccl_5/136-2212818-9687203?psc=1</t>
   </si>
   <si>
     <t>Use a cabeça! Python ― 2ª edição</t>
@@ -404,7 +401,7 @@
     <t>R$ 121,44</t>
   </si>
   <si>
-    <t>amazon.com.br/Use-Cabe%C3%A7a-Python-2%C2%AA-Edi%C3%A7%C3%A3o/dp/8550803405/ref=zg_mw_g_7842670011_sccl_6/145-7952979-0205767?psc=1</t>
+    <t>amazon.com.br/Use-Cabe%C3%A7a-Python-2%C2%AA-Edi%C3%A7%C3%A3o/dp/8550803405/ref=zg_mw_g_7842670011_sccl_6/136-2212818-9687203?psc=1</t>
   </si>
   <si>
     <t>Java efetivo: as melhores práticas para a plataforma Java</t>
@@ -416,7 +413,7 @@
     <t>R$ 117,00</t>
   </si>
   <si>
-    <t>amazon.com.br/Java-Efetivo-Melhores-Pr%C3%A1ticas-Plataforma/dp/8550804622/ref=zg_mw_g_7842670011_sccl_7/145-7952979-0205767?psc=1</t>
+    <t>amazon.com.br/Java-Efetivo-Melhores-Pr%C3%A1ticas-Plataforma/dp/8550804622/ref=zg_mw_g_7842670011_sccl_7/136-2212818-9687203?psc=1</t>
   </si>
   <si>
     <t>Scrum - Um Guia de Bolso: Um companheiro de viagem inteligente</t>
@@ -428,7 +425,7 @@
     <t>R$ 24,99</t>
   </si>
   <si>
-    <t>amazon.com.br/Scrum-Bolso-companheiro-viagem-inteligente-ebook/dp/B07TDN99LX/ref=zg_mw_g_7842670011_sccl_8/145-7952979-0205767?psc=1</t>
+    <t>amazon.com.br/Scrum-Bolso-companheiro-viagem-inteligente-ebook/dp/B07TDN99LX/ref=zg_mw_g_7842670011_sccl_8/136-2212818-9687203?psc=1</t>
   </si>
   <si>
     <t>Problemas Clássicos de Ciência da Computação com Python</t>
@@ -440,7 +437,7 @@
     <t>R$ 68,66</t>
   </si>
   <si>
-    <t>amazon.com.br/Problemas-Cl%C3%A1ssicos-Ci%C3%AAncia-Computa%C3%A7%C3%A3o-Python/dp/8575228056/ref=zg_mw_g_7842670011_sccl_9/145-7952979-0205767?psc=1</t>
+    <t>amazon.com.br/Problemas-Cl%C3%A1ssicos-Ci%C3%AAncia-Computa%C3%A7%C3%A3o-Python/dp/8575228056/ref=zg_mw_g_7842670011_sccl_9/136-2212818-9687203?psc=1</t>
   </si>
   <si>
     <t>Entrega Contínua: Como Entregar Software de Forma Rápida e ConfiávelJez Humble</t>
@@ -452,7 +449,7 @@
     <t>R$ 180,00</t>
   </si>
   <si>
-    <t>amazon.com.br/Entrega-Cont%C3%ADnua-Entregar-Software-Confi%C3%A1vel-ebook/dp/B016LFWKG4/ref=zg_mw_g_7842670011_sccl_10/145-7952979-0205767?psc=1</t>
+    <t>amazon.com.br/Entrega-Cont%C3%ADnua-Entregar-Software-Confi%C3%A1vel-ebook/dp/B016LFWKG4/ref=zg_mw_g_7842670011_sccl_10/136-2212818-9687203?psc=1</t>
   </si>
   <si>
     <t>Pentest em Aplicações web</t>
@@ -464,7 +461,7 @@
     <t>R$ 102,49</t>
   </si>
   <si>
-    <t>amazon.com.br/Pentest-Aplica%C3%A7%C3%B5es-Web-Daniel-Moreno/dp/8575226134/ref=zg_mw_g_7842670011_sccl_11/145-7952979-0205767?psc=1</t>
+    <t>amazon.com.br/Pentest-Aplica%C3%A7%C3%B5es-Web-Daniel-Moreno/dp/8575226134/ref=zg_mw_g_7842670011_sccl_11/136-2212818-9687203?psc=1</t>
   </si>
   <si>
     <t>Matemática com Python: Um Guia PráticoGuilherme A. Barucke Marcondes</t>
@@ -476,7 +473,7 @@
     <t>R$ 49,60</t>
   </si>
   <si>
-    <t>amazon.com.br/Matem%C3%A1tica-com-Python-Guia-Pr%C3%A1tico-ebook/dp/B07J32H1DB/ref=zg_mw_g_7842670011_sccl_12/145-7952979-0205767?psc=1</t>
+    <t>amazon.com.br/Matem%C3%A1tica-com-Python-Guia-Pr%C3%A1tico-ebook/dp/B07J32H1DB/ref=zg_mw_g_7842670011_sccl_12/136-2212818-9687203?psc=1</t>
   </si>
   <si>
     <t>Aprendendo Node: Usando JavaScript no Servidor</t>
@@ -488,7 +485,7 @@
     <t>R$ 92,00</t>
   </si>
   <si>
-    <t>amazon.com.br/Aprendendo-Node-Usando-JavaScript-Servidor/dp/8575225405/ref=zg_mw_g_7842670011_sccl_13/145-7952979-0205767?psc=1</t>
+    <t>amazon.com.br/Aprendendo-Node-Usando-JavaScript-Servidor/dp/8575225405/ref=zg_mw_g_7842670011_sccl_13/136-2212818-9687203?psc=1</t>
   </si>
   <si>
     <t>Use a cabeça! Padrões de projetos (Design Patterns): padrões de projetos</t>
@@ -500,7 +497,7 @@
     <t>R$ 200,16</t>
   </si>
   <si>
-    <t>amazon.com.br/Cabe%C3%A7a-Padr%C3%B5es-Projetos-Eric-Freeman/dp/8576081741/ref=zg_mw_g_7842670011_sccl_14/145-7952979-0205767?psc=1</t>
+    <t>amazon.com.br/Cabe%C3%A7a-Padr%C3%B5es-Projetos-Eric-Freeman/dp/8576081741/ref=zg_mw_g_7842670011_sccl_14/136-2212818-9687203?psc=1</t>
   </si>
   <si>
     <t>Pense em Python: Pense como um cientista da computaçãoAllen B. Downey</t>
@@ -509,7 +506,7 @@
     <t>R$ 76,00</t>
   </si>
   <si>
-    <t>amazon.com.br/Pense-Python-como-cientista-computa%C3%A7%C3%A3o-ebook/dp/B07QL2LKBG/ref=zg_mw_g_7842670011_sccl_15/145-7952979-0205767?psc=1</t>
+    <t>amazon.com.br/Pense-Python-como-cientista-computa%C3%A7%C3%A3o-ebook/dp/B07QL2LKBG/ref=zg_mw_g_7842670011_sccl_15/136-2212818-9687203?psc=1</t>
   </si>
   <si>
     <t>1001 videogames para jogar antes de morrer</t>
@@ -518,7 +515,7 @@
     <t>Tony Mott</t>
   </si>
   <si>
-    <t>amazon.com.br/1001-videogames-jogar-antes-morrer/dp/8575429191/ref=zg_mw_g_7842670011_sccl_16/145-7952979-0205767?psc=1</t>
+    <t>amazon.com.br/1001-videogames-jogar-antes-morrer/dp/8575429191/ref=zg_mw_g_7842670011_sccl_16/136-2212818-9687203?psc=1</t>
   </si>
   <si>
     <t>Design digital: conceitos e aplicações para websites, animações, vídeos e webgamesFabiana Guerra</t>
@@ -530,7 +527,7 @@
     <t>R$ 60,53</t>
   </si>
   <si>
-    <t>amazon.com.br/Design-digital-conceitos-aplica%C3%A7%C3%B5es-anima%C3%A7%C3%B5es/dp/8539626969/ref=zg_mw_g_7842670011_sccl_17/145-7952979-0205767?psc=1</t>
+    <t>amazon.com.br/Design-digital-conceitos-aplica%C3%A7%C3%B5es-anima%C3%A7%C3%B5es/dp/8539626969/ref=zg_mw_g_7842670011_sccl_17/136-2212818-9687203?psc=1</t>
   </si>
   <si>
     <t>A Linguagem de Programação GoAlan A. A. Donovan</t>
@@ -542,7 +539,7 @@
     <t>R$ 84,80</t>
   </si>
   <si>
-    <t>amazon.com.br/Linguagem-Programa%C3%A7%C3%A3o-Go-Alan-Donovan/dp/8575225464/ref=zg_mw_g_7842670011_sccl_18/145-7952979-0205767?psc=1</t>
+    <t>amazon.com.br/Linguagem-Programa%C3%A7%C3%A3o-Go-Alan-Donovan/dp/8575225464/ref=zg_mw_g_7842670011_sccl_18/136-2212818-9687203?psc=1</t>
   </si>
   <si>
     <t>Como ser um programador melhor: Um manual para programadores que se importam com código</t>
@@ -554,7 +551,7 @@
     <t>R$ 79,20</t>
   </si>
   <si>
-    <t>amazon.com.br/Como-ser-programador-melhor-programadores-ebook/dp/B07S7F6RCW/ref=zg_mw_g_7842670011_sccl_19/145-7952979-0205767?psc=1</t>
+    <t>amazon.com.br/Como-ser-programador-melhor-programadores-ebook/dp/B07S7F6RCW/ref=zg_mw_g_7842670011_sccl_19/136-2212818-9687203?psc=1</t>
   </si>
   <si>
     <t>Criando apps para empresas com Android</t>
@@ -563,7 +560,7 @@
     <t>R$ 9,90</t>
   </si>
   <si>
-    <t>amazon.com.br/Criando-apps-para-empresas-Android-ebook/dp/B01IJQ0AU6/ref=zg_mw_g_7842670011_sccl_20/145-7952979-0205767?psc=1</t>
+    <t>amazon.com.br/Criando-apps-para-empresas-Android-ebook/dp/B01IJQ0AU6/ref=zg_mw_g_7842670011_sccl_20/136-2212818-9687203?psc=1</t>
   </si>
   <si>
     <t>Algoritmos: Lógica Para Desenvolvimento de Programação de Computadores - Edição Revisada e AtualizadaJosé Augusto N. G. Manzano</t>
@@ -575,7 +572,7 @@
     <t>R$ 58,99</t>
   </si>
   <si>
-    <t>amazon.com.br/Algoritmos-Desenvolvimento-Programa%C3%A7%C3%A3o-Computadores-Atualizada/dp/8536531452/ref=zg_mw_g_7842670011_sccl_21/145-7952979-0205767?psc=1</t>
+    <t>amazon.com.br/Algoritmos-Desenvolvimento-Programa%C3%A7%C3%A3o-Computadores-Atualizada/dp/8536531452/ref=zg_mw_g_7842670011_sccl_21/136-2212818-9687203?psc=1</t>
   </si>
   <si>
     <t>Jornada DevOps: unindo cultura ágil, Lean e tecnologia para entrega de software de qualidade (Jornada Colaborativa)Antonio Muniz</t>
@@ -587,7 +584,7 @@
     <t>R$ 28,50</t>
   </si>
   <si>
-    <t>amazon.com.br/Jornada-DevOps-tecnologia-software-qualidade-ebook/dp/B07S4FFJTJ/ref=zg_mw_g_7842670011_sccl_22/145-7952979-0205767?psc=1</t>
+    <t>amazon.com.br/Jornada-DevOps-tecnologia-software-qualidade-ebook/dp/B07S4FFJTJ/ref=zg_mw_g_7842670011_sccl_22/136-2212818-9687203?psc=1</t>
   </si>
   <si>
     <t>Shell Script Profissional</t>
@@ -599,7 +596,7 @@
     <t>R$ 76,99</t>
   </si>
   <si>
-    <t>amazon.com.br/Script-Profissional-Aurelio-Marinho-Jargas/dp/8575221523/ref=zg_mw_g_7842670011_sccl_24/145-7952979-0205767?psc=1</t>
+    <t>amazon.com.br/Script-Profissional-Aurelio-Marinho-Jargas/dp/8575221523/ref=zg_mw_g_7842670011_sccl_24/136-2212818-9687203?psc=1</t>
   </si>
   <si>
     <t>Desmistificando algoritmosThomas Cormen</t>
@@ -608,7 +605,7 @@
     <t>Thomas Cormen</t>
   </si>
   <si>
-    <t>amazon.com.br/Desmistificando-Algoritmos-Thomas-H-Cormen/dp/8535271775/ref=zg_mw_g_7842670011_sccl_25/145-7952979-0205767?psc=1</t>
+    <t>amazon.com.br/Desmistificando-Algoritmos-Thomas-H-Cormen/dp/8535271775/ref=zg_mw_g_7842670011_sccl_25/136-2212818-9687203?psc=1</t>
   </si>
   <si>
     <t>Desenvolvimento web com Flask: Desenvolvendo Aplicações web com Python</t>
@@ -617,7 +614,7 @@
     <t>Miguel Grinberg</t>
   </si>
   <si>
-    <t>amazon.com.br/Desenvolvimento-Web-com-Flask-Desenvolvendo/dp/8575226819/ref=zg_mw_g_7842670011_sccl_27/145-7952979-0205767?psc=1</t>
+    <t>amazon.com.br/Desenvolvimento-Web-com-Flask-Desenvolvendo/dp/8575226819/ref=zg_mw_g_7842670011_sccl_27/136-2212818-9687203?psc=1</t>
   </si>
   <si>
     <t>O Programador Pragmático: De Aprendiz a Mestre</t>
@@ -629,7 +626,7 @@
     <t>R$ 155,20</t>
   </si>
   <si>
-    <t>amazon.com.br/Programador-Pragm%C3%A1tico-Aprendiz-Mestre-ebook/dp/B019HM0H90/ref=zg_mw_g_7842670011_sccl_28/145-7952979-0205767?psc=1</t>
+    <t>amazon.com.br/Programador-Pragm%C3%A1tico-Aprendiz-Mestre-ebook/dp/B019HM0H90/ref=zg_mw_g_7842670011_sccl_28/136-2212818-9687203?psc=1</t>
   </si>
   <si>
     <t>O Programador Apaixonado: Construindo uma carreira notável em desenvolvimento de softwareChad Fowler</t>
@@ -638,7 +635,7 @@
     <t>Chad Fowler</t>
   </si>
   <si>
-    <t>amazon.com.br/Programador-Apaixonado-Construindo-carreira-desenvolvimento-ebook/dp/B00VAAM7LE/ref=zg_mw_g_7842670011_sccl_29/145-7952979-0205767?psc=1</t>
+    <t>amazon.com.br/Programador-Apaixonado-Construindo-carreira-desenvolvimento-ebook/dp/B00VAAM7LE/ref=zg_mw_g_7842670011_sccl_29/136-2212818-9687203?psc=1</t>
   </si>
   <si>
     <t>Aprendendo Padrões de Projeto em Python: Tire Proveito da Eficácia dos Padrões de Projeto (design Patterns) em Python Para Resolver Problemas do Mundo Real em Arquitetura e Design de Software</t>
@@ -647,10 +644,10 @@
     <t>Chetan Giridhar</t>
   </si>
   <si>
-    <t>R$ 60,60</t>
-  </si>
-  <si>
-    <t>amazon.com.br/Aprendendo-Padr%C3%B5es-Projeto-Python-Arquitetura/dp/8575225235/ref=zg_mw_g_7842670011_sccl_30/145-7952979-0205767?psc=1</t>
+    <t>R$ 57,40</t>
+  </si>
+  <si>
+    <t>amazon.com.br/Aprendendo-Padr%C3%B5es-Projeto-Python-Arquitetura/dp/8575225235/ref=zg_mw_g_7842670011_sccl_30/136-2212818-9687203?psc=1</t>
   </si>
 </sst>
 </file>
@@ -1286,24 +1283,24 @@
         <v>88</v>
       </c>
       <c r="C24" t="s">
+        <v>42</v>
+      </c>
+      <c r="D24" t="s">
         <v>89</v>
-      </c>
-      <c r="D24" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
+        <v>90</v>
+      </c>
+      <c r="B25" t="s">
         <v>91</v>
       </c>
-      <c r="B25" t="s">
+      <c r="C25" t="s">
         <v>92</v>
       </c>
-      <c r="C25" t="s">
+      <c r="D25" t="s">
         <v>93</v>
-      </c>
-      <c r="D25" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="26">
@@ -1314,472 +1311,472 @@
         <v>69</v>
       </c>
       <c r="C26" t="s">
+        <v>94</v>
+      </c>
+      <c r="D26" t="s">
         <v>95</v>
-      </c>
-      <c r="D26" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
+        <v>96</v>
+      </c>
+      <c r="B27" t="s">
         <v>97</v>
-      </c>
-      <c r="B27" t="s">
-        <v>98</v>
       </c>
       <c r="C27" t="s">
         <v>70</v>
       </c>
       <c r="D27" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
+        <v>99</v>
+      </c>
+      <c r="B28" t="s">
         <v>100</v>
       </c>
-      <c r="B28" t="s">
+      <c r="C28" t="s">
         <v>101</v>
       </c>
-      <c r="C28" t="s">
+      <c r="D28" t="s">
         <v>102</v>
-      </c>
-      <c r="D28" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
+        <v>103</v>
+      </c>
+      <c r="B29" t="s">
         <v>104</v>
       </c>
-      <c r="B29" t="s">
-        <v>105</v>
-      </c>
       <c r="C29" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D29" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B30" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C30" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D30" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B31" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C31" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D31" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
+        <v>107</v>
+      </c>
+      <c r="B32" t="s">
         <v>108</v>
       </c>
-      <c r="B32" t="s">
+      <c r="C32" t="s">
         <v>109</v>
       </c>
-      <c r="C32" t="s">
+      <c r="D32" t="s">
         <v>110</v>
-      </c>
-      <c r="D32" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
+        <v>111</v>
+      </c>
+      <c r="B33" t="s">
         <v>112</v>
       </c>
-      <c r="B33" t="s">
+      <c r="C33" t="s">
         <v>113</v>
       </c>
-      <c r="C33" t="s">
+      <c r="D33" t="s">
         <v>114</v>
-      </c>
-      <c r="D33" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
+        <v>115</v>
+      </c>
+      <c r="B34" t="s">
         <v>116</v>
       </c>
-      <c r="B34" t="s">
+      <c r="C34" t="s">
         <v>117</v>
       </c>
-      <c r="C34" t="s">
+      <c r="D34" t="s">
         <v>118</v>
-      </c>
-      <c r="D34" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
+        <v>119</v>
+      </c>
+      <c r="B35" t="s">
         <v>120</v>
       </c>
-      <c r="B35" t="s">
+      <c r="C35" t="s">
         <v>121</v>
       </c>
-      <c r="C35" t="s">
+      <c r="D35" t="s">
         <v>122</v>
-      </c>
-      <c r="D35" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
+        <v>119</v>
+      </c>
+      <c r="B36" t="s">
         <v>120</v>
       </c>
-      <c r="B36" t="s">
-        <v>121</v>
-      </c>
       <c r="C36" t="s">
+        <v>123</v>
+      </c>
+      <c r="D36" t="s">
         <v>124</v>
-      </c>
-      <c r="D36" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
+        <v>125</v>
+      </c>
+      <c r="B37" t="s">
         <v>126</v>
       </c>
-      <c r="B37" t="s">
+      <c r="C37" t="s">
         <v>127</v>
       </c>
-      <c r="C37" t="s">
+      <c r="D37" t="s">
         <v>128</v>
-      </c>
-      <c r="D37" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
+        <v>129</v>
+      </c>
+      <c r="B38" t="s">
         <v>130</v>
       </c>
-      <c r="B38" t="s">
+      <c r="C38" t="s">
         <v>131</v>
       </c>
-      <c r="C38" t="s">
+      <c r="D38" t="s">
         <v>132</v>
-      </c>
-      <c r="D38" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
+        <v>133</v>
+      </c>
+      <c r="B39" t="s">
         <v>134</v>
       </c>
-      <c r="B39" t="s">
+      <c r="C39" t="s">
         <v>135</v>
       </c>
-      <c r="C39" t="s">
+      <c r="D39" t="s">
         <v>136</v>
-      </c>
-      <c r="D39" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
+        <v>137</v>
+      </c>
+      <c r="B40" t="s">
         <v>138</v>
       </c>
-      <c r="B40" t="s">
+      <c r="C40" t="s">
         <v>139</v>
       </c>
-      <c r="C40" t="s">
+      <c r="D40" t="s">
         <v>140</v>
-      </c>
-      <c r="D40" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
+        <v>141</v>
+      </c>
+      <c r="B41" t="s">
         <v>142</v>
       </c>
-      <c r="B41" t="s">
+      <c r="C41" t="s">
         <v>143</v>
       </c>
-      <c r="C41" t="s">
+      <c r="D41" t="s">
         <v>144</v>
-      </c>
-      <c r="D41" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
+        <v>145</v>
+      </c>
+      <c r="B42" t="s">
         <v>146</v>
       </c>
-      <c r="B42" t="s">
+      <c r="C42" t="s">
         <v>147</v>
       </c>
-      <c r="C42" t="s">
+      <c r="D42" t="s">
         <v>148</v>
-      </c>
-      <c r="D42" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
+        <v>149</v>
+      </c>
+      <c r="B43" t="s">
         <v>150</v>
       </c>
-      <c r="B43" t="s">
+      <c r="C43" t="s">
         <v>151</v>
       </c>
-      <c r="C43" t="s">
+      <c r="D43" t="s">
         <v>152</v>
-      </c>
-      <c r="D43" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
+        <v>153</v>
+      </c>
+      <c r="B44" t="s">
         <v>154</v>
       </c>
-      <c r="B44" t="s">
+      <c r="C44" t="s">
         <v>155</v>
       </c>
-      <c r="C44" t="s">
+      <c r="D44" t="s">
         <v>156</v>
-      </c>
-      <c r="D44" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
+        <v>157</v>
+      </c>
+      <c r="B45" t="s">
         <v>158</v>
       </c>
-      <c r="B45" t="s">
+      <c r="C45" t="s">
         <v>159</v>
       </c>
-      <c r="C45" t="s">
+      <c r="D45" t="s">
         <v>160</v>
-      </c>
-      <c r="D45" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B46" t="s">
         <v>73</v>
       </c>
       <c r="C46" t="s">
+        <v>162</v>
+      </c>
+      <c r="D46" t="s">
         <v>163</v>
-      </c>
-      <c r="D46" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
+        <v>164</v>
+      </c>
+      <c r="B47" t="s">
         <v>165</v>
       </c>
-      <c r="B47" t="s">
+      <c r="C47" t="s">
+        <v>104</v>
+      </c>
+      <c r="D47" t="s">
         <v>166</v>
-      </c>
-      <c r="C47" t="s">
-        <v>105</v>
-      </c>
-      <c r="D47" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
+        <v>167</v>
+      </c>
+      <c r="B48" t="s">
         <v>168</v>
       </c>
-      <c r="B48" t="s">
+      <c r="C48" t="s">
         <v>169</v>
       </c>
-      <c r="C48" t="s">
+      <c r="D48" t="s">
         <v>170</v>
-      </c>
-      <c r="D48" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
+        <v>171</v>
+      </c>
+      <c r="B49" t="s">
         <v>172</v>
       </c>
-      <c r="B49" t="s">
+      <c r="C49" t="s">
         <v>173</v>
       </c>
-      <c r="C49" t="s">
+      <c r="D49" t="s">
         <v>174</v>
-      </c>
-      <c r="D49" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
+        <v>175</v>
+      </c>
+      <c r="B50" t="s">
         <v>176</v>
       </c>
-      <c r="B50" t="s">
+      <c r="C50" t="s">
         <v>177</v>
       </c>
-      <c r="C50" t="s">
+      <c r="D50" t="s">
         <v>178</v>
-      </c>
-      <c r="D50" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B51" t="s">
         <v>21</v>
       </c>
       <c r="C51" t="s">
+        <v>180</v>
+      </c>
+      <c r="D51" t="s">
         <v>181</v>
-      </c>
-      <c r="D51" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
+        <v>182</v>
+      </c>
+      <c r="B52" t="s">
         <v>183</v>
       </c>
-      <c r="B52" t="s">
+      <c r="C52" t="s">
         <v>184</v>
       </c>
-      <c r="C52" t="s">
+      <c r="D52" t="s">
         <v>185</v>
-      </c>
-      <c r="D52" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
+        <v>186</v>
+      </c>
+      <c r="B53" t="s">
         <v>187</v>
       </c>
-      <c r="B53" t="s">
+      <c r="C53" t="s">
         <v>188</v>
       </c>
-      <c r="C53" t="s">
+      <c r="D53" t="s">
         <v>189</v>
-      </c>
-      <c r="D53" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
+        <v>190</v>
+      </c>
+      <c r="B54" t="s">
         <v>191</v>
       </c>
-      <c r="B54" t="s">
+      <c r="C54" t="s">
         <v>192</v>
       </c>
-      <c r="C54" t="s">
+      <c r="D54" t="s">
         <v>193</v>
-      </c>
-      <c r="D54" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
+        <v>194</v>
+      </c>
+      <c r="B55" t="s">
         <v>195</v>
       </c>
-      <c r="B55" t="s">
+      <c r="C55" t="s">
+        <v>104</v>
+      </c>
+      <c r="D55" t="s">
         <v>196</v>
-      </c>
-      <c r="C55" t="s">
-        <v>105</v>
-      </c>
-      <c r="D55" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
+        <v>197</v>
+      </c>
+      <c r="B56" t="s">
         <v>198</v>
       </c>
-      <c r="B56" t="s">
+      <c r="C56" t="s">
+        <v>104</v>
+      </c>
+      <c r="D56" t="s">
         <v>199</v>
-      </c>
-      <c r="C56" t="s">
-        <v>105</v>
-      </c>
-      <c r="D56" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s">
+        <v>200</v>
+      </c>
+      <c r="B57" t="s">
         <v>201</v>
       </c>
-      <c r="B57" t="s">
+      <c r="C57" t="s">
         <v>202</v>
       </c>
-      <c r="C57" t="s">
+      <c r="D57" t="s">
         <v>203</v>
-      </c>
-      <c r="D57" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s">
+        <v>204</v>
+      </c>
+      <c r="B58" t="s">
         <v>205</v>
-      </c>
-      <c r="B58" t="s">
-        <v>206</v>
       </c>
       <c r="C58" t="s">
         <v>70</v>
       </c>
       <c r="D58" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s">
+        <v>207</v>
+      </c>
+      <c r="B59" t="s">
         <v>208</v>
       </c>
-      <c r="B59" t="s">
+      <c r="C59" t="s">
         <v>209</v>
       </c>
-      <c r="C59" t="s">
+      <c r="D59" t="s">
         <v>210</v>
-      </c>
-      <c r="D59" t="s">
-        <v>211</v>
       </c>
     </row>
   </sheetData>

</xml_diff>